<commit_message>
add some submodules with external MCP servers
</commit_message>
<xml_diff>
--- a/information_sources.xlsx
+++ b/information_sources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sheldonmrampton/Documents/Code/shellbot2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99CBDDFC-FE12-A442-B056-BDA9D01219EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFB1713C-646B-F846-A09D-FD4503B8FDA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="1000" windowWidth="26980" windowHeight="14360" xr2:uid="{8888E50F-C287-474A-8994-390D35653B18}"/>
+    <workbookView xWindow="1100" yWindow="1020" windowWidth="26980" windowHeight="14360" xr2:uid="{8888E50F-C287-474A-8994-390D35653B18}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="91">
   <si>
     <t>MS Word, PDF and other documents stored on Sheldon's laptop</t>
   </si>
@@ -300,6 +300,15 @@
   </si>
   <si>
     <t>Monthly</t>
+  </si>
+  <si>
+    <t>MVP done</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Write only!</t>
   </si>
 </sst>
 </file>
@@ -692,10 +701,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3FFC382-A200-624D-BD8B-7A3D11D3F24D}">
-  <dimension ref="A1:K39"/>
+  <dimension ref="A1:L39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -703,11 +712,11 @@
     <col min="1" max="1" width="56.1640625" customWidth="1"/>
     <col min="2" max="2" width="10.33203125" customWidth="1"/>
     <col min="3" max="3" width="15.83203125" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" style="3"/>
-    <col min="10" max="10" width="16.33203125" customWidth="1"/>
+    <col min="10" max="10" width="10.83203125" style="3"/>
+    <col min="11" max="11" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>33</v>
       </c>
@@ -721,28 +730,31 @@
         <v>35</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -756,28 +768,31 @@
         <v>73</v>
       </c>
       <c r="E2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F2" t="s">
         <v>74</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>72</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>75</v>
       </c>
-      <c r="H2" t="s">
-        <v>70</v>
-      </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" t="s">
+        <v>70</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>77</v>
       </c>
-      <c r="K2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="L2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -791,28 +806,31 @@
         <v>73</v>
       </c>
       <c r="E3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F3" t="s">
         <v>74</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>72</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>79</v>
       </c>
-      <c r="H3" t="s">
-        <v>70</v>
-      </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" t="s">
+        <v>70</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>77</v>
       </c>
-      <c r="K3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="L3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -822,69 +840,72 @@
       <c r="C4" t="s">
         <v>49</v>
       </c>
-      <c r="G4" t="s">
+      <c r="E4" t="s">
+        <v>89</v>
+      </c>
+      <c r="H4" t="s">
         <v>81</v>
       </c>
-      <c r="H4" t="s">
-        <v>70</v>
-      </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" t="s">
+        <v>70</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>77</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
         <v>49</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>78</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>80</v>
       </c>
-      <c r="H5" t="s">
-        <v>70</v>
-      </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" t="s">
+        <v>70</v>
+      </c>
+      <c r="J5" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>82</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
         <v>50</v>
       </c>
-      <c r="H6" t="s">
-        <v>70</v>
-      </c>
-      <c r="K6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I6" t="s">
+        <v>70</v>
+      </c>
+      <c r="L6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -894,14 +915,14 @@
       <c r="C7" t="s">
         <v>51</v>
       </c>
-      <c r="H7" t="s">
-        <v>70</v>
-      </c>
-      <c r="K7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I7" t="s">
+        <v>70</v>
+      </c>
+      <c r="L7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -911,14 +932,17 @@
       <c r="C8" t="s">
         <v>51</v>
       </c>
-      <c r="H8" t="s">
-        <v>70</v>
-      </c>
-      <c r="K8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E8" t="s">
+        <v>90</v>
+      </c>
+      <c r="I8" t="s">
+        <v>70</v>
+      </c>
+      <c r="L8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -928,14 +952,14 @@
       <c r="C9" t="s">
         <v>52</v>
       </c>
-      <c r="H9" t="s">
-        <v>70</v>
-      </c>
-      <c r="K9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I9" t="s">
+        <v>70</v>
+      </c>
+      <c r="L9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -945,14 +969,17 @@
       <c r="C10" t="s">
         <v>53</v>
       </c>
-      <c r="H10" t="s">
-        <v>70</v>
-      </c>
-      <c r="K10" t="s">
+      <c r="E10" t="s">
+        <v>89</v>
+      </c>
+      <c r="I10" t="s">
+        <v>70</v>
+      </c>
+      <c r="L10" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -962,14 +989,14 @@
       <c r="C11" t="s">
         <v>54</v>
       </c>
-      <c r="H11" t="s">
-        <v>70</v>
-      </c>
-      <c r="K11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I11" t="s">
+        <v>70</v>
+      </c>
+      <c r="L11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -979,14 +1006,14 @@
       <c r="C12" t="s">
         <v>55</v>
       </c>
-      <c r="H12" t="s">
-        <v>70</v>
-      </c>
-      <c r="K12" t="s">
+      <c r="I12" t="s">
+        <v>70</v>
+      </c>
+      <c r="L12" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -996,14 +1023,14 @@
       <c r="C13" t="s">
         <v>50</v>
       </c>
-      <c r="H13" t="s">
-        <v>70</v>
-      </c>
-      <c r="K13" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I13" t="s">
+        <v>70</v>
+      </c>
+      <c r="L13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1013,14 +1040,14 @@
       <c r="C14" t="s">
         <v>50</v>
       </c>
-      <c r="H14" t="s">
-        <v>70</v>
-      </c>
-      <c r="K14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I14" t="s">
+        <v>70</v>
+      </c>
+      <c r="L14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1030,14 +1057,17 @@
       <c r="C15" t="s">
         <v>56</v>
       </c>
-      <c r="H15" t="s">
-        <v>70</v>
-      </c>
-      <c r="K15" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E15" t="s">
+        <v>89</v>
+      </c>
+      <c r="I15" t="s">
+        <v>70</v>
+      </c>
+      <c r="L15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>57</v>
       </c>
@@ -1047,14 +1077,14 @@
       <c r="C16" t="s">
         <v>50</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
         <v>71</v>
       </c>
-      <c r="K16" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -1064,14 +1094,14 @@
       <c r="C17" t="s">
         <v>50</v>
       </c>
-      <c r="H17" t="s">
-        <v>70</v>
-      </c>
-      <c r="K17" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I17" t="s">
+        <v>70</v>
+      </c>
+      <c r="L17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -1081,14 +1111,14 @@
       <c r="C18" t="s">
         <v>51</v>
       </c>
-      <c r="H18" t="s">
-        <v>70</v>
-      </c>
-      <c r="K18" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I18" t="s">
+        <v>70</v>
+      </c>
+      <c r="L18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -1098,14 +1128,14 @@
       <c r="C19" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H19" t="s">
-        <v>70</v>
-      </c>
-      <c r="K19" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I19" t="s">
+        <v>70</v>
+      </c>
+      <c r="L19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -1115,14 +1145,14 @@
       <c r="C20" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H20" t="s">
-        <v>70</v>
-      </c>
-      <c r="K20" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I20" t="s">
+        <v>70</v>
+      </c>
+      <c r="L20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -1132,14 +1162,14 @@
       <c r="C21" t="s">
         <v>58</v>
       </c>
-      <c r="H21" t="s">
-        <v>70</v>
-      </c>
-      <c r="K21" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I21" t="s">
+        <v>70</v>
+      </c>
+      <c r="L21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -1149,14 +1179,14 @@
       <c r="C22" t="s">
         <v>59</v>
       </c>
-      <c r="H22" t="s">
-        <v>70</v>
-      </c>
-      <c r="K22" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I22" t="s">
+        <v>70</v>
+      </c>
+      <c r="L22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -1166,14 +1196,17 @@
       <c r="C23" t="s">
         <v>60</v>
       </c>
-      <c r="H23" t="s">
-        <v>70</v>
-      </c>
-      <c r="K23" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E23" t="s">
+        <v>89</v>
+      </c>
+      <c r="I23" t="s">
+        <v>70</v>
+      </c>
+      <c r="L23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -1183,14 +1216,17 @@
       <c r="C24" t="s">
         <v>61</v>
       </c>
-      <c r="H24" t="s">
-        <v>70</v>
-      </c>
-      <c r="K24" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E24" t="s">
+        <v>89</v>
+      </c>
+      <c r="I24" t="s">
+        <v>70</v>
+      </c>
+      <c r="L24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -1200,14 +1236,14 @@
       <c r="C25" t="s">
         <v>48</v>
       </c>
-      <c r="H25" t="s">
-        <v>70</v>
-      </c>
-      <c r="K25" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I25" t="s">
+        <v>70</v>
+      </c>
+      <c r="L25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -1217,14 +1253,14 @@
       <c r="C26" t="s">
         <v>48</v>
       </c>
-      <c r="H26" t="s">
-        <v>70</v>
-      </c>
-      <c r="K26" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I26" t="s">
+        <v>70</v>
+      </c>
+      <c r="L26" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>24</v>
       </c>
@@ -1234,14 +1270,14 @@
       <c r="C27" t="s">
         <v>48</v>
       </c>
-      <c r="H27" t="s">
-        <v>70</v>
-      </c>
-      <c r="K27" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I27" t="s">
+        <v>70</v>
+      </c>
+      <c r="L27" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>25</v>
       </c>
@@ -1251,14 +1287,14 @@
       <c r="C28" t="s">
         <v>62</v>
       </c>
-      <c r="H28" t="s">
-        <v>70</v>
-      </c>
-      <c r="K28" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I28" t="s">
+        <v>70</v>
+      </c>
+      <c r="L28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>26</v>
       </c>
@@ -1268,14 +1304,14 @@
       <c r="C29" t="s">
         <v>63</v>
       </c>
-      <c r="H29" t="s">
-        <v>70</v>
-      </c>
-      <c r="K29" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I29" t="s">
+        <v>70</v>
+      </c>
+      <c r="L29" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>27</v>
       </c>
@@ -1285,14 +1321,14 @@
       <c r="C30" t="s">
         <v>64</v>
       </c>
-      <c r="H30" t="s">
-        <v>70</v>
-      </c>
-      <c r="K30" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I30" t="s">
+        <v>70</v>
+      </c>
+      <c r="L30" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>28</v>
       </c>
@@ -1302,14 +1338,14 @@
       <c r="C31" t="s">
         <v>64</v>
       </c>
-      <c r="H31" t="s">
-        <v>70</v>
-      </c>
-      <c r="K31" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I31" t="s">
+        <v>70</v>
+      </c>
+      <c r="L31" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>29</v>
       </c>
@@ -1319,14 +1355,14 @@
       <c r="C32" t="s">
         <v>65</v>
       </c>
-      <c r="H32" t="s">
-        <v>70</v>
-      </c>
-      <c r="K32" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I32" t="s">
+        <v>70</v>
+      </c>
+      <c r="L32" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>30</v>
       </c>
@@ -1336,14 +1372,14 @@
       <c r="C33" t="s">
         <v>66</v>
       </c>
-      <c r="H33" t="s">
-        <v>70</v>
-      </c>
-      <c r="K33" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I33" t="s">
+        <v>70</v>
+      </c>
+      <c r="L33" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>31</v>
       </c>
@@ -1353,14 +1389,14 @@
       <c r="C34" t="s">
         <v>69</v>
       </c>
-      <c r="H34" t="s">
-        <v>70</v>
-      </c>
-      <c r="K34" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I34" t="s">
+        <v>70</v>
+      </c>
+      <c r="L34" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>32</v>
       </c>
@@ -1370,14 +1406,17 @@
       <c r="C35" t="s">
         <v>67</v>
       </c>
-      <c r="H35" t="s">
-        <v>70</v>
-      </c>
-      <c r="K35" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E35" t="s">
+        <v>89</v>
+      </c>
+      <c r="I35" t="s">
+        <v>70</v>
+      </c>
+      <c r="L35" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>45</v>
       </c>
@@ -1387,14 +1426,14 @@
       <c r="C36" t="s">
         <v>68</v>
       </c>
-      <c r="H36" t="s">
+      <c r="I36" t="s">
         <v>71</v>
       </c>
-      <c r="K36" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L36" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>46</v>
       </c>
@@ -1404,14 +1443,14 @@
       <c r="C37" t="s">
         <v>68</v>
       </c>
-      <c r="H37" t="s">
-        <v>70</v>
-      </c>
-      <c r="K37" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I37" t="s">
+        <v>70</v>
+      </c>
+      <c r="L37" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>47</v>
       </c>
@@ -1421,14 +1460,14 @@
       <c r="C38" t="s">
         <v>68</v>
       </c>
-      <c r="H38" t="s">
-        <v>70</v>
-      </c>
-      <c r="K38" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I38" t="s">
+        <v>70</v>
+      </c>
+      <c r="L38" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>84</v>
       </c>
@@ -1438,10 +1477,10 @@
       <c r="C39" t="s">
         <v>85</v>
       </c>
-      <c r="H39" t="s">
+      <c r="I39" t="s">
         <v>86</v>
       </c>
-      <c r="K39" t="s">
+      <c r="L39" t="s">
         <v>87</v>
       </c>
     </row>

</xml_diff>